<commit_message>
Final habitación baile listo
</commit_message>
<xml_diff>
--- a/faltantes.xlsx
+++ b/faltantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Esteban VC\Proyectos\Unity\Depresion2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AC733B-4398-4D9B-A8F9-7AF81C6CF963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF0DBAD-CD47-4C04-8F95-379647D096DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3925E70F-A77C-46A1-9CDA-085D93446D3E}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="C3:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,26 +704,26 @@
       <c r="C25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D26" t="s">
+      <c r="D26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D27" t="s">
+      <c r="D27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="7" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rompecabezas de partituras integradas
habitación 1 casi lista
</commit_message>
<xml_diff>
--- a/faltantes.xlsx
+++ b/faltantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Esteban VC\Proyectos\Unity\Depresion2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF0DBAD-CD47-4C04-8F95-379647D096DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586ED7DA-B469-42A7-8350-F6EA77B85633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3925E70F-A77C-46A1-9CDA-085D93446D3E}"/>
   </bookViews>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2559096D-37C6-46B2-B8F5-9FA370727FCE}">
   <dimension ref="C3:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,10 +588,10 @@
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -604,10 +604,10 @@
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -623,10 +623,10 @@
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
+      <c r="D13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="7" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correción de bugs en la escena 1.4
</commit_message>
<xml_diff>
--- a/faltantes.xlsx
+++ b/faltantes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Esteban VC\Proyectos\Unity\Depresion2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586ED7DA-B469-42A7-8350-F6EA77B85633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B277AD-70F6-44C8-AFE1-9667238D01C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3925E70F-A77C-46A1-9CDA-085D93446D3E}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="C3:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,34 +669,34 @@
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
+      <c r="D21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D22" t="s">
+      <c r="D22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D23" t="s">
+      <c r="D23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="7" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>